<commit_message>
Conditional formatting file updated
</commit_message>
<xml_diff>
--- a/XLOOKUP Excel Tutorial File.xlsx
+++ b/XLOOKUP Excel Tutorial File.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sadiqunnurayan/Documents/GitHub/Excel-Learning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{344CFC44-6AC6-4605-AA55-CB25FF348249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{008BE20C-64A3-D347-AF1C-5E7C6D736869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5EA44D8F-79D3-45F5-A0F6-C7F47358B7ED}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" activeTab="2" xr2:uid="{5EA44D8F-79D3-45F5-A0F6-C7F47358B7ED}"/>
   </bookViews>
   <sheets>
     <sheet name="XLookUp" sheetId="1" r:id="rId1"/>
@@ -693,19 +693,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1027015F-D30F-450C-928C-DE78480974B7}">
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="24.5546875" customWidth="1"/>
+    <col min="2" max="2" width="24.5" customWidth="1"/>
     <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="40.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E1" t="s">
         <v>0</v>
       </c>
@@ -743,7 +743,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>60</v>
       </c>
@@ -784,7 +784,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>65</v>
       </c>
@@ -826,7 +826,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -868,7 +868,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -910,7 +910,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>69</v>
       </c>
@@ -952,7 +952,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E7">
         <v>1006</v>
       </c>
@@ -987,7 +987,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E8">
         <v>1007</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E9">
         <v>1008</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E10">
         <v>1009</v>
       </c>
@@ -1092,13 +1092,13 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H22" t="str">
         <f t="shared" ref="H22:H23" si="1">CONCATENATE(F12," ",G12)</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="23" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H23" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
@@ -1114,19 +1114,19 @@
   <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5546875" customWidth="1"/>
+    <col min="3" max="3" width="24.5" customWidth="1"/>
     <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="40.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="F1" t="s">
         <v>0</v>
       </c>
@@ -1161,7 +1161,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>60</v>
       </c>
@@ -1205,7 +1205,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>65</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -1340,7 +1340,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>69</v>
       </c>
@@ -1385,7 +1385,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="F7">
         <v>1006</v>
       </c>
@@ -1420,7 +1420,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="F8">
         <v>1007</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="F9">
         <v>1008</v>
       </c>
@@ -1490,7 +1490,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="F10">
         <v>1009</v>
       </c>
@@ -1525,13 +1525,13 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I22" t="str">
         <f t="shared" ref="I22:I23" si="0">CONCATENATE(G12," ",H12)</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="23" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I23" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
@@ -1546,20 +1546,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32A7D64C-38C9-4586-AD37-471BFBE38708}">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" customWidth="1"/>
+    <col min="2" max="2" width="24.5" customWidth="1"/>
     <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="40.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E1" t="s">
         <v>0</v>
       </c>
@@ -1594,7 +1594,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>60</v>
       </c>
@@ -1635,13 +1635,13 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>86</v>
       </c>
       <c r="B3" t="str">
-        <f>_xlfn.XLOOKUP(A3,H2:H10,O2:O10,"Not Found",2)</f>
-        <v>Not Found</v>
+        <f>_xlfn.XLOOKUP(A3&amp;"*",H2:H10,O2:O10,"Not Found",2)</f>
+        <v>Toby.Flenderson@DunderMifflinCorporate.com</v>
       </c>
       <c r="E3">
         <v>1002</v>
@@ -1677,7 +1677,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -1761,7 +1761,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>87</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E7">
         <v>1006</v>
       </c>
@@ -1838,7 +1838,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E8">
         <v>1007</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E9">
         <v>1008</v>
       </c>
@@ -1908,7 +1908,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E10">
         <v>1009</v>
       </c>
@@ -1943,13 +1943,13 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H22" t="str">
         <f t="shared" ref="H22:H23" si="0">CONCATENATE(F12," ",G12)</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="23" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H23" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
@@ -1965,20 +1965,20 @@
   <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.77734375" customWidth="1"/>
-    <col min="3" max="3" width="24.5546875" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="24.5" customWidth="1"/>
     <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="40.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="F1" t="s">
         <v>0</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>88</v>
       </c>
@@ -2054,7 +2054,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>90</v>
       </c>
@@ -2096,7 +2096,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>38</v>
       </c>
@@ -2138,7 +2138,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="F5">
         <v>1004</v>
       </c>
@@ -2173,7 +2173,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="F6">
         <v>1005</v>
       </c>
@@ -2208,7 +2208,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="F7">
         <v>1006</v>
       </c>
@@ -2243,7 +2243,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="F8">
         <v>1007</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="F9">
         <v>1008</v>
       </c>
@@ -2313,7 +2313,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="F10">
         <v>1009</v>
       </c>
@@ -2348,13 +2348,13 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I22" t="str">
         <f t="shared" ref="I22:I23" si="0">CONCATENATE(G12," ",H12)</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="23" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I23" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
@@ -2373,12 +2373,12 @@
       <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>73</v>
       </c>
@@ -2419,7 +2419,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -2467,7 +2467,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>71</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -2576,12 +2576,12 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>73</v>
       </c>
@@ -2622,7 +2622,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -2670,7 +2670,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>71</v>
       </c>
@@ -2718,7 +2718,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -2766,12 +2766,12 @@
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>70</v>
       </c>
@@ -2789,16 +2789,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8F9C169-12D8-441E-870D-6C6EF0F6521C}">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B5"/>
+    <sheetView zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E1" t="s">
         <v>0</v>
       </c>
@@ -2836,7 +2837,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>60</v>
       </c>
@@ -2877,7 +2878,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>63</v>
       </c>
@@ -2919,7 +2920,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>66</v>
       </c>
@@ -2961,7 +2962,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>68</v>
       </c>
@@ -3003,7 +3004,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E6">
         <v>1005</v>
       </c>
@@ -3038,7 +3039,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E7">
         <v>1006</v>
       </c>
@@ -3073,7 +3074,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E8">
         <v>1007</v>
       </c>
@@ -3108,7 +3109,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E9">
         <v>1008</v>
       </c>
@@ -3143,7 +3144,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E10">
         <v>1009</v>
       </c>

</xml_diff>